<commit_message>
Add FA A2 Information. Peak Value A2FA
</commit_message>
<xml_diff>
--- a/DividendAndCGSummary2025.xlsx
+++ b/DividendAndCGSummary2025.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD3BE68-A158-4A27-A888-C7599E7BB9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF31C2D-CD7D-4E13-AC45-8A9603762C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{8BEB55FD-3D38-4AA2-9725-6750C9DA47E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{8BEB55FD-3D38-4AA2-9725-6750C9DA47E5}"/>
   </bookViews>
   <sheets>
     <sheet name="RSU" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="160">
   <si>
     <t>Year</t>
   </si>
@@ -483,9 +505,6 @@
     <t>&gt;Download Etrade ClientStatements between April 2024 to March 2025. Search Qualified Dividend in each sheet. Fill Qualified Dividend and  Tax Withholding in column M and N,  Validate the date from that statement</t>
   </si>
   <si>
-    <t>&gt;Download RSU Reports From My Reports ADP and Paste as it is col A:O. Fill Sellable Quantity col P from Etrade -&gt; Holdings -&gt; Sellable.  Drag rest of the column sample to autopopulate.</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;Download ESPP Reports From My Reports ADP and Paste as it is col A:L. Repeat to auto fill remaining. </t>
   </si>
   <si>
@@ -505,6 +524,24 @@
   </si>
   <si>
     <t>Tax @ 31.24</t>
+  </si>
+  <si>
+    <t>Compute Manually for Schedule A2</t>
+  </si>
+  <si>
+    <t>Peak Balance</t>
+  </si>
+  <si>
+    <t>Peak Balance as all remaining shares on peak day after getting last shares. i.e 4 Dec 2024. Depending on stocks on</t>
+  </si>
+  <si>
+    <t>Closing Balance</t>
+  </si>
+  <si>
+    <t>Proceed from Sale</t>
+  </si>
+  <si>
+    <t>&gt;Optional : Download RSU Reports From My Reports ADP and Paste as it is col A:O. Fill Sellable Quantity col P from Etrade -&gt; Holdings -&gt; Sellable.  Drag rest of the column sample to autopopulate.</t>
   </si>
 </sst>
 </file>
@@ -895,7 +932,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1048,6 +1085,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1095,7 +1147,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1204,6 +1256,13 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,13 +1308,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1702,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB2A4CB-5922-42AD-9312-C77D74614993}">
   <dimension ref="A1:Y100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1737,22 +1801,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="39" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
@@ -1768,19 +1832,19 @@
       <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="32">
         <v>0</v>
       </c>
@@ -1810,12 +1874,12 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="33">
         <f>SUM(N8:N10,N11)</f>
         <v>0</v>
@@ -1845,12 +1909,12 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="9">
         <f>CEILING(L2-L3,1)</f>
         <v>0</v>
@@ -2031,7 +2095,7 @@
       <c r="I8" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J8" s="41">
         <v>45463</v>
       </c>
       <c r="K8">
@@ -2094,7 +2158,7 @@
       <c r="I9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="41">
         <v>45561</v>
       </c>
       <c r="K9">
@@ -2146,20 +2210,20 @@
       <c r="Y9" s="15"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="38"/>
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="41">
         <v>45645</v>
       </c>
       <c r="K10">
@@ -2197,8 +2261,8 @@
         <v>54</v>
       </c>
       <c r="U10">
-        <f>0.04*0.33</f>
-        <v>1.3200000000000002E-2</v>
+        <f>0.04*0.3</f>
+        <v>1.2E-2</v>
       </c>
       <c r="V10" s="9">
         <f>$S$8*U10</f>
@@ -2209,18 +2273,18 @@
       <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="38"/>
       <c r="I11" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="57">
+      <c r="J11" s="41">
         <v>45743</v>
       </c>
       <c r="K11">
@@ -2259,7 +2323,7 @@
       </c>
       <c r="U11">
         <f>SUM(U8:U10)</f>
-        <v>0.31319999999999998</v>
+        <v>0.312</v>
       </c>
       <c r="V11" s="9">
         <f>$S$8*U11</f>
@@ -2276,20 +2340,20 @@
       <c r="Y11" s="15"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
+      <c r="A12" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
@@ -2863,20 +2927,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="A1" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
     </row>
     <row r="2" spans="1:21" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3114,7 +3178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E98C5B-0A34-4C05-8055-756E485EBFF6}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -3142,14 +3206,14 @@
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3244,27 +3308,27 @@
       <c r="N3" s="8">
         <v>123.09400799999992</v>
       </c>
-      <c r="Q3" s="50" t="s">
+      <c r="Q3" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -3291,10 +3355,10 @@
         <v>19</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>92</v>
@@ -3310,7 +3374,7 @@
         <v>95</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>98</v>
@@ -3327,7 +3391,7 @@
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -3395,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9A6A94-A28D-49A0-9E93-E290917C2700}">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3430,30 +3494,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="39" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="56"/>
       <c r="U1" s="15"/>
       <c r="V1" s="15"/>
       <c r="W1" s="15"/>
@@ -3461,30 +3527,30 @@
       <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="21">
         <v>58</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="56"/>
       <c r="U2" s="15"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
@@ -3503,24 +3569,24 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="21">
         <f>SUM(N8:N10,N11)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="56"/>
       <c r="U3" s="15"/>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
@@ -3539,12 +3605,12 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="21">
         <f>L2-L3</f>
         <v>58</v>
@@ -3586,18 +3652,20 @@
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
+      <c r="M5" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="44"/>
       <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -3704,16 +3772,16 @@
         <v>42</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="21" t="s">
-        <v>72</v>
+      <c r="C8" s="17">
+        <v>45292</v>
       </c>
       <c r="D8" s="17">
         <v>45461</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="39">
         <v>227.09</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="39">
         <v>83.12</v>
       </c>
       <c r="G8" s="21">
@@ -3777,16 +3845,18 @@
       <c r="Y8" s="15"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="53"/>
+      <c r="C9" s="17">
+        <v>45342</v>
+      </c>
+      <c r="D9" s="17">
+        <v>45461</v>
+      </c>
+      <c r="E9" s="39">
+        <v>227.09</v>
+      </c>
+      <c r="F9" s="39">
+        <v>83.12</v>
+      </c>
       <c r="I9" s="21" t="s">
         <v>36</v>
       </c>
@@ -3842,14 +3912,18 @@
       <c r="Y9" s="15"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="53"/>
+      <c r="C10" s="17">
+        <v>45432</v>
+      </c>
+      <c r="D10" s="17">
+        <v>45461</v>
+      </c>
+      <c r="E10" s="39">
+        <v>227.09</v>
+      </c>
+      <c r="F10" s="39">
+        <v>83.12</v>
+      </c>
       <c r="I10" s="21" t="s">
         <v>37</v>
       </c>
@@ -3903,14 +3977,18 @@
       <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="53"/>
+      <c r="C11" s="17">
+        <v>45524</v>
+      </c>
+      <c r="D11" s="17">
+        <v>45579</v>
+      </c>
+      <c r="E11" s="39">
+        <v>178.04</v>
+      </c>
+      <c r="F11" s="39">
+        <v>83.66</v>
+      </c>
       <c r="I11" s="21" t="s">
         <v>38</v>
       </c>
@@ -3965,25 +4043,23 @@
       </c>
       <c r="X11" s="21">
         <f>SUM($Y:$Y)</f>
-        <v>725.47279999999955</v>
+        <v>555.1487999999996</v>
       </c>
       <c r="Y11" s="15"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
+      <c r="C12" s="17">
+        <v>45616</v>
+      </c>
+      <c r="D12" s="17">
+        <v>45630</v>
+      </c>
+      <c r="E12" s="39">
+        <v>163.34</v>
+      </c>
+      <c r="F12" s="39">
+        <v>84.3</v>
+      </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
@@ -4128,8 +4204,8 @@
         <f>ROUND(N14-O14, 0)</f>
         <v>1081100</v>
       </c>
-      <c r="R14" s="21">
-        <f>ROUND(FA!$E$8*FA!$F$8*P14,0)</f>
+      <c r="R14" s="21" cm="1">
+        <f t="array" ref="R14">ROUND(_xlfn.LET(_xlpm.peak_after, MATCH(MIN(IF($C$8:$C$12&gt;=T14, $C$8:$C$12)), $C$8:$C$12, 0), INDEX($E$8:$E$12, _xlpm.peak_after) * INDEX($F$8:$F$12, _xlpm.peak_after)) *P14, 0)</f>
         <v>566272</v>
       </c>
       <c r="S14" s="21">
@@ -4436,20 +4512,20 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
+      <c r="E25" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
       <c r="Q25"/>
       <c r="R25"/>
       <c r="S25"/>
@@ -4526,11 +4602,11 @@
       </c>
     </row>
     <row r="27" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
       <c r="E27" s="2">
         <v>12312</v>
       </c>
@@ -4544,7 +4620,7 @@
         <v>76</v>
       </c>
       <c r="I27" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J27" s="2">
         <v>112.3445</v>
@@ -4553,7 +4629,7 @@
         <v>148.51</v>
       </c>
       <c r="L27" s="2">
-        <v>325.49</v>
+        <v>41</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>25</v>
@@ -4562,14 +4638,14 @@
         <v>82.78</v>
       </c>
       <c r="O27" s="2">
-        <v>26944.0622</v>
+        <v>123</v>
       </c>
       <c r="P27" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Q27" s="21">
         <f>ROUND(P27*K27*N27, 0)</f>
-        <v>110643</v>
+        <v>24587</v>
       </c>
       <c r="R27" s="21">
         <v>136422</v>
@@ -4583,31 +4659,31 @@
       </c>
       <c r="U27" s="21">
         <f>IF($T27&lt;FA!$J$8,1,0)*FA!$K$8*P27</f>
-        <v>7.2</v>
+        <v>1.6</v>
       </c>
       <c r="V27" s="21">
         <f>ROUND((IF($T27&lt;FA!$J$8,1,0)*FA!$K$8*FA!$L$8)*$P27, 0)</f>
-        <v>594</v>
+        <v>132</v>
       </c>
       <c r="W27" s="21">
         <f>0.25*V27</f>
-        <v>148.5</v>
+        <v>33</v>
       </c>
       <c r="X27" s="21">
         <f>0.3132*V27</f>
-        <v>186.04079999999999</v>
+        <v>41.342399999999998</v>
       </c>
       <c r="Y27" s="21">
         <f>X27-W27</f>
-        <v>37.54079999999999</v>
+        <v>8.3423999999999978</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
       <c r="E28" s="2">
         <v>12312</v>
       </c>
@@ -4621,7 +4697,7 @@
         <v>76</v>
       </c>
       <c r="I28" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
         <v>112.3445</v>
@@ -4630,7 +4706,7 @@
         <v>148.51</v>
       </c>
       <c r="L28" s="2">
-        <v>325.49</v>
+        <v>12</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>25</v>
@@ -4639,22 +4715,22 @@
         <v>82.78</v>
       </c>
       <c r="O28" s="2">
-        <v>26944.0622</v>
+        <v>12312</v>
       </c>
       <c r="P28" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="28">
         <f>ROUND(P28*K28*N28, 0)</f>
-        <v>110643</v>
-      </c>
-      <c r="R28" s="28">
-        <f>ROUND(E8*F8*P28, 0)</f>
-        <v>169881</v>
+        <v>12294</v>
+      </c>
+      <c r="R28" s="28" cm="1">
+        <f t="array" ref="R28">ROUND(_xlfn.LET(_xlpm.peak_after, MATCH(MIN(IF($C$8:$C$12&gt;=T28, $C$8:$C$12)), $C$8:$C$12, 0), INDEX($E$8:$E$12, _xlpm.peak_after) * INDEX($F$8:$F$12, _xlpm.peak_after)) *P28, 0)</f>
+        <v>18876</v>
       </c>
       <c r="S28" s="28">
         <f>ROUND(G8*H8*P28, 0)</f>
-        <v>117796</v>
+        <v>13088</v>
       </c>
       <c r="T28" s="10">
         <f>DATE(VALUE(RIGHT(H28,4)), IFERROR(VALUE(LEFT(H28,2)), VALUE(LEFT(H28,1))), IFERROR(VALUE(MID(H28,3,2)),VALUE(MID(H28,4,2))))</f>
@@ -4662,23 +4738,23 @@
       </c>
       <c r="U28" s="28">
         <f>IF($T28&lt;FA!$J$8,1,0)*FA!$K$8*P28 + IF($T28&lt;FA!$J$9,1,0)*FA!$K$9*P28 + IF($T28&lt;FA!$J$10,1,0)*FA!$K$10*P28 + IF($T28&lt;FA!$J$11,1,0)*FA!$K$11*P28</f>
-        <v>30.15</v>
+        <v>3.35</v>
       </c>
       <c r="V28" s="28">
         <f>ROUND((IF($T28&lt;FA!$J$8,1,0)*FA!$K$8*FA!$L$8 + IF($T28&lt;FA!$J$9,1,0)*FA!$K$9*FA!$L$9 + IF($T28&lt;FA!$J$10,1,0)*FA!$K$10*FA!$L$10 + IF($T28&lt;FA!$J$11,1,0)*FA!$K$11*FA!$L$11)*$P28, 0)</f>
-        <v>2512</v>
+        <v>279</v>
       </c>
       <c r="W28" s="28">
         <f>0.25*V28</f>
-        <v>628</v>
+        <v>69.75</v>
       </c>
       <c r="X28" s="28">
         <f>0.3132*V28</f>
-        <v>786.75839999999994</v>
+        <v>87.382799999999989</v>
       </c>
       <c r="Y28" s="28">
         <f>X28-W28</f>
-        <v>158.75839999999994</v>
+        <v>17.632799999999989</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
@@ -4689,44 +4765,99 @@
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q33" s="15"/>
     </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="60"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="40">
+        <f>ROUND(SUM(O17:O25,O31) * D15 * E15, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+    </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
+      <c r="A37" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="40">
+        <f>SUM(R17:R25,R30:R31)</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
       <c r="J37"/>
       <c r="K37"/>
       <c r="L37"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38" s="26"/>
-      <c r="H38"/>
-      <c r="I38"/>
+      <c r="A38" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="40">
+        <v>19180</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
       <c r="J38"/>
       <c r="K38"/>
       <c r="L38"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39" s="26"/>
-      <c r="H39"/>
-      <c r="I39"/>
+      <c r="A39" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="40">
+        <v>136422</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
       <c r="J39"/>
       <c r="K39"/>
       <c r="L39"/>
@@ -4738,7 +4869,7 @@
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
-      <c r="G40" s="26"/>
+      <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -4858,8 +4989,10 @@
       <c r="L48"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A12:L12"/>
+  <mergeCells count="12">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="M5:X5"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="E25:P25"/>
     <mergeCell ref="A27:C27"/>
@@ -4868,7 +5001,7 @@
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A9:H11"/>
+    <mergeCell ref="M1:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="X11">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
@@ -4912,11 +5045,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
@@ -4932,14 +5065,14 @@
       <c r="G2" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
@@ -4948,9 +5081,9 @@
       <c r="C4" s="30"/>
       <c r="E4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
@@ -4959,18 +5092,18 @@
       <c r="C5" s="30"/>
       <c r="E5" s="30"/>
       <c r="G5" s="30"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27"/>
       <c r="C6" s="31"/>
       <c r="E6" s="31"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
@@ -4979,11 +5112,11 @@
       <c r="C7" s="31"/>
       <c r="E7" s="30"/>
       <c r="G7" s="30"/>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
@@ -4992,11 +5125,11 @@
       <c r="C8" s="31"/>
       <c r="E8" s="30"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
@@ -5005,18 +5138,18 @@
       <c r="C9" s="31"/>
       <c r="E9" s="31"/>
       <c r="G9" s="30"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="C10" s="31"/>
       <c r="E10" s="31"/>
       <c r="G10" s="30"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
@@ -5025,11 +5158,11 @@
       <c r="C11" s="30"/>
       <c r="E11" s="30"/>
       <c r="G11" s="30"/>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
@@ -5038,18 +5171,18 @@
       <c r="C12" s="30"/>
       <c r="E12" s="30"/>
       <c r="G12" s="30"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="C13" s="31"/>
       <c r="E13" s="31"/>
       <c r="G13" s="30"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
@@ -5058,11 +5191,11 @@
       <c r="C14" s="30"/>
       <c r="E14" s="30"/>
       <c r="G14" s="30"/>
-      <c r="H14" s="54" t="s">
+      <c r="H14" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
@@ -5071,11 +5204,11 @@
       <c r="C15" s="31"/>
       <c r="E15" s="31"/>
       <c r="G15" s="30"/>
-      <c r="H15" s="54" t="s">
+      <c r="H15" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27" t="s">
@@ -5084,9 +5217,9 @@
       <c r="C16" s="30"/>
       <c r="E16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
@@ -5095,11 +5228,11 @@
       <c r="C17" s="31"/>
       <c r="E17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54" t="s">
+      <c r="H17" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
@@ -5108,11 +5241,11 @@
       <c r="C18" s="30"/>
       <c r="E18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54" t="s">
+      <c r="H18" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
@@ -5121,20 +5254,20 @@
       <c r="C19" s="31"/>
       <c r="E19" s="31"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="C20" s="31"/>
       <c r="E20" s="31"/>
       <c r="G20" s="30"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27" t="s">
@@ -5143,9 +5276,9 @@
       <c r="C21" s="30"/>
       <c r="E21" s="30"/>
       <c r="G21" s="30"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27" t="s">
@@ -5154,9 +5287,9 @@
       <c r="C22" s="30"/>
       <c r="E22" s="30"/>
       <c r="G22" s="30"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
     </row>
     <row r="23" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
@@ -5165,20 +5298,21 @@
       <c r="C23" s="31"/>
       <c r="E23" s="30"/>
       <c r="G23" s="30"/>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
@@ -5191,12 +5325,11 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add average tax rate. FA Schedule A2 calculation.
</commit_message>
<xml_diff>
--- a/DividendAndCGSummary2025.xlsx
+++ b/DividendAndCGSummary2025.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF31C2D-CD7D-4E13-AC45-8A9603762C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6381A6E3-12B1-4D76-A3F7-51F853A37054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{8BEB55FD-3D38-4AA2-9725-6750C9DA47E5}"/>
+    <workbookView xWindow="372" yWindow="1392" windowWidth="30912" windowHeight="12120" xr2:uid="{8BEB55FD-3D38-4AA2-9725-6750C9DA47E5}"/>
   </bookViews>
   <sheets>
     <sheet name="RSU" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
   <si>
     <t>Year</t>
   </si>
@@ -523,18 +523,12 @@
     <t>Sell Price Per Unit</t>
   </si>
   <si>
-    <t>Tax @ 31.24</t>
-  </si>
-  <si>
     <t>Compute Manually for Schedule A2</t>
   </si>
   <si>
     <t>Peak Balance</t>
   </si>
   <si>
-    <t>Peak Balance as all remaining shares on peak day after getting last shares. i.e 4 Dec 2024. Depending on stocks on</t>
-  </si>
-  <si>
     <t>Closing Balance</t>
   </si>
   <si>
@@ -542,6 +536,27 @@
   </si>
   <si>
     <t>&gt;Optional : Download RSU Reports From My Reports ADP and Paste as it is col A:O. Fill Sellable Quantity col P from Etrade -&gt; Holdings -&gt; Sellable.  Drag rest of the column sample to autopopulate.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Fill all income values in a ITR utlity without claiming relief or in a income tax calculator to get total income and total tax. I got my average tax as 21.56%</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Average Rate of  Tax %</t>
+  </si>
+  <si>
+    <t>Tax payable on such income under normal provisions in India (d) . For Dividend. Average Rate of Tax * Total Dividend</t>
+  </si>
+  <si>
+    <t>Tax @ 30</t>
+  </si>
+  <si>
+    <t>Peak Balance as all remaining shares on peak day after getting last shares. i.e 4 Dec 2024.</t>
   </si>
 </sst>
 </file>
@@ -932,7 +947,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1100,6 +1115,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1147,7 +1201,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1215,20 +1269,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="12" fillId="6" borderId="5" xfId="10" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1253,16 +1297,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1296,29 +1346,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="6" borderId="5" xfId="10" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1766,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB2A4CB-5922-42AD-9312-C77D74614993}">
   <dimension ref="A1:Y100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1801,30 +1875,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="42" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="15"/>
       <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="S1" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" s="59" t="s">
+        <v>119</v>
+      </c>
       <c r="U1" s="15"/>
       <c r="V1" s="15"/>
       <c r="W1" s="15"/>
@@ -1832,37 +1910,43 @@
       <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="42" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="32">
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="28">
         <v>0</v>
       </c>
       <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="60">
+        <v>100</v>
+      </c>
       <c r="U2" s="15"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
     </row>
-    <row r="3" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
@@ -1874,30 +1958,35 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="33">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="29">
         <f>SUM(N8:N10,N11)</f>
         <v>0</v>
       </c>
       <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="60">
+        <v>10</v>
+      </c>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -1909,34 +1998,36 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
       <c r="L4" s="9">
         <f>CEILING(L2-L3,1)</f>
         <v>0</v>
       </c>
       <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="V4" s="15"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="T4" s="59">
+        <f>T3/T2</f>
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="72" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -1955,15 +2046,24 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
+      <c r="N5" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="R5" s="52"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="59">
+        <f>ROUND(T4 *S8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
@@ -1986,8 +2086,6 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
       <c r="S6" s="15"/>
@@ -2046,10 +2144,10 @@
       <c r="Q7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="R7" s="37" t="s">
+      <c r="R7" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="S7" s="37" t="s">
+      <c r="S7" s="33" t="s">
         <v>104</v>
       </c>
       <c r="T7" s="16" t="s">
@@ -2058,10 +2156,10 @@
       <c r="U7" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="V7" s="37" t="s">
+      <c r="V7" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="W7" s="37" t="s">
+      <c r="W7" s="33" t="s">
         <v>57</v>
       </c>
       <c r="X7" s="16" t="s">
@@ -2095,7 +2193,7 @@
       <c r="I8" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="35">
         <v>45463</v>
       </c>
       <c r="K8">
@@ -2122,10 +2220,10 @@
         <f>0.3132*O8</f>
         <v>0</v>
       </c>
-      <c r="R8" s="34" t="s">
+      <c r="R8" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="31">
         <f>ROUND(SUM((O8:O11)), 0)</f>
         <v>0</v>
       </c>
@@ -2149,16 +2247,16 @@
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="I9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="35">
         <v>45561</v>
       </c>
       <c r="K9">
@@ -2185,10 +2283,10 @@
         <f t="shared" ref="Q9:Q11" si="2">0.3132*O9</f>
         <v>0</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="R9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="S9" s="36">
+      <c r="S9" s="32">
         <f>SUM(M8:M11)</f>
         <v>0</v>
       </c>
@@ -2210,20 +2308,20 @@
       <c r="Y9" s="15"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="38"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="34"/>
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="35">
         <v>45645</v>
       </c>
       <c r="K10">
@@ -2250,10 +2348,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="34" t="s">
+      <c r="R10" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="35">
+      <c r="S10" s="31">
         <f>SUM((P8:P11))</f>
         <v>0</v>
       </c>
@@ -2273,18 +2371,18 @@
       <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="38"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="34"/>
       <c r="I11" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="35">
         <v>45743</v>
       </c>
       <c r="K11">
@@ -2311,10 +2409,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R11" s="34" t="s">
+      <c r="R11" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="S11" s="36">
+      <c r="S11" s="32">
         <f>SUM(N8:N11)</f>
         <v>0</v>
       </c>
@@ -2340,20 +2438,20 @@
       <c r="Y11" s="15"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
+      <c r="A12" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
@@ -2479,7 +2577,7 @@
       <c r="K14" s="11">
         <v>1</v>
       </c>
-      <c r="L14" s="29" t="s">
+      <c r="L14" s="25" t="s">
         <v>143</v>
       </c>
       <c r="M14" s="11" t="s">
@@ -2861,7 +2959,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="O2:R3"/>
+    <mergeCell ref="Q5:S5"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H4:K4"/>
@@ -2927,20 +3027,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:21" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3179,7 +3279,7 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3206,14 +3306,14 @@
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3308,27 +3408,27 @@
       <c r="N3" s="8">
         <v>123.09400799999992</v>
       </c>
-      <c r="Q3" s="53" t="s">
+      <c r="Q3" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -3391,7 +3491,7 @@
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -3440,8 +3540,8 @@
       </c>
       <c r="O8" s="12"/>
       <c r="P8" s="12">
-        <f>N8*0.3124</f>
-        <v>2149.2951303999994</v>
+        <f>N8*0.3</f>
+        <v>2063.9837999999995</v>
       </c>
     </row>
   </sheetData>
@@ -3459,67 +3559,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9A6A94-A28D-49A0-9E93-E290917C2700}">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.44140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5546875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="25.77734375" style="38" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="17" style="38" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="38" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="38" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="38" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" style="38" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="38" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="38" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" style="38" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="38" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="38" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" style="38" customWidth="1"/>
+    <col min="17" max="17" width="15" style="38" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" style="38" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" style="38" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" style="38" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" style="38" customWidth="1"/>
+    <col min="22" max="22" width="14" style="38" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" style="38" customWidth="1"/>
+    <col min="24" max="24" width="8.5546875" style="38" customWidth="1"/>
+    <col min="25" max="25" width="12.5546875" style="38" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="42" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="48" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="56"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="55"/>
       <c r="U1" s="15"/>
       <c r="V1" s="15"/>
       <c r="W1" s="15"/>
@@ -3527,30 +3627,30 @@
       <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="42" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="21">
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="36">
         <v>58</v>
       </c>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="56"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="55"/>
       <c r="U2" s="15"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
@@ -3569,31 +3669,31 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="21">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="36">
         <f>SUM(N8:N10,N11)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="56"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="55"/>
       <c r="U3" s="15"/>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -3605,29 +3705,27 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="21">
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="36">
         <f>L2-L3</f>
         <v>58</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+      <c r="M4" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="36" t="s">
+        <v>81</v>
+      </c>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
-      <c r="T4" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>81</v>
-      </c>
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
@@ -3645,27 +3743,27 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="43" t="s">
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="42"/>
       <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -3778,28 +3876,28 @@
       <c r="D8" s="17">
         <v>45461</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="36">
         <v>227.09</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="36">
         <v>83.12</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="36">
         <v>153.62</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="36">
         <v>85.2</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="65">
         <v>45372</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="23">
         <v>0.8</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="66">
         <v>82.49</v>
       </c>
       <c r="M8" s="18">
@@ -3808,40 +3906,40 @@
       <c r="N8" s="18">
         <v>0</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="36">
         <f>M8*L9</f>
         <v>0</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="36">
         <f>VALUE(N8)*L9</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="36">
         <f>0.3132*O8</f>
         <v>0</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="36">
         <f>SUM((O8:O11))</f>
         <v>0</v>
       </c>
       <c r="S8" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="36">
         <v>0.3</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="36">
         <f>R8*U8</f>
         <v>0</v>
       </c>
-      <c r="W8" s="21">
+      <c r="W8" s="36">
         <f>V11</f>
         <v>0</v>
       </c>
-      <c r="X8" s="21"/>
+      <c r="X8" s="36"/>
       <c r="Y8" s="15"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
@@ -3851,22 +3949,22 @@
       <c r="D9" s="17">
         <v>45461</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="36">
         <v>227.09</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="36">
         <v>83.12</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="36" t="s">
         <v>36</v>
       </c>
       <c r="J9" s="17">
         <v>45463</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="36">
         <v>0.85</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="36">
         <v>83.05</v>
       </c>
       <c r="M9" s="18">
@@ -3875,15 +3973,15 @@
       <c r="N9" s="18">
         <v>0</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="36">
         <f>M9*L10</f>
         <v>0</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="36">
         <f>VALUE(N9)*L10</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="36">
         <f t="shared" ref="Q9:Q11" si="0">0.3132*O9</f>
         <v>0</v>
       </c>
@@ -3894,21 +3992,21 @@
       <c r="S9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="U9" s="21">
-        <v>0</v>
-      </c>
-      <c r="V9" s="21">
+      <c r="U9" s="36">
+        <v>0</v>
+      </c>
+      <c r="V9" s="36">
         <f>$R$8*U9</f>
         <v>0</v>
       </c>
-      <c r="W9" s="21">
+      <c r="W9" s="36">
         <f>SUM(P8:P11)</f>
         <v>0</v>
       </c>
-      <c r="X9" s="21"/>
+      <c r="X9" s="36"/>
       <c r="Y9" s="15"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
@@ -3918,22 +4016,22 @@
       <c r="D10" s="17">
         <v>45461</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="36">
         <v>227.09</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <v>83.12</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="36" t="s">
         <v>37</v>
       </c>
       <c r="J10" s="17">
         <v>45561</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="36">
         <v>0.85</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="36">
         <v>83.5</v>
       </c>
       <c r="M10" s="18">
@@ -3942,38 +4040,38 @@
       <c r="N10" s="18">
         <v>0</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="36">
         <f>M10*L11</f>
         <v>0</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="36">
         <f>VALUE(N10)*L11</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="36">
         <f>SUM((P8:P11))</f>
         <v>0</v>
       </c>
       <c r="S10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="T10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="36">
         <f>0.04*0.33</f>
         <v>1.3200000000000002E-2</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="36">
         <f>$R$8*U10</f>
         <v>0</v>
       </c>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
       <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -3983,39 +4081,39 @@
       <c r="D11" s="17">
         <v>45579</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="36">
         <v>178.04</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="36">
         <v>83.66</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="36" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="17">
         <v>45645</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="36">
         <v>0.85</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="36">
         <v>84.15</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M11" s="23">
         <v>0</v>
       </c>
       <c r="N11" s="18">
         <v>0</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="36">
         <f>M11*L8</f>
         <v>0</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="36">
         <f>VALUE(N11)*L8</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4026,22 +4124,22 @@
       <c r="S11" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="T11" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="U11" s="21">
+      <c r="U11" s="36">
         <f>SUM(U8:U10)</f>
         <v>0.31319999999999998</v>
       </c>
-      <c r="V11" s="21">
+      <c r="V11" s="36">
         <f>$R$8*U11</f>
         <v>0</v>
       </c>
-      <c r="W11" s="21">
+      <c r="W11" s="36">
         <f>V11-SUM(P8:P11)</f>
         <v>0</v>
       </c>
-      <c r="X11" s="21">
+      <c r="X11" s="36">
         <f>SUM($Y:$Y)</f>
         <v>555.1487999999996</v>
       </c>
@@ -4054,10 +4152,10 @@
       <c r="D12" s="17">
         <v>45630</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="36">
         <v>163.34</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="36">
         <v>84.3</v>
       </c>
       <c r="M12" s="15"/>
@@ -4152,63 +4250,63 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="37">
         <v>12312</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="15">
         <v>100</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="15">
         <v>100</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="15">
         <v>34.32</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="15">
         <v>1</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="15">
         <v>1</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="15">
         <v>10</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="15">
         <v>2312312</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="15">
         <v>1231212</v>
       </c>
-      <c r="P14" s="11">
+      <c r="P14" s="15">
         <v>30</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="36">
         <f>ROUND(N14-O14, 0)</f>
         <v>1081100</v>
       </c>
-      <c r="R14" s="21" cm="1">
+      <c r="R14" s="36" cm="1">
         <f t="array" ref="R14">ROUND(_xlfn.LET(_xlpm.peak_after, MATCH(MIN(IF($C$8:$C$12&gt;=T14, $C$8:$C$12)), $C$8:$C$12, 0), INDEX($E$8:$E$12, _xlpm.peak_after) * INDEX($F$8:$F$12, _xlpm.peak_after)) *P14, 0)</f>
         <v>566272</v>
       </c>
-      <c r="S14" s="21">
+      <c r="S14" s="36">
         <f>ROUND(FA!$G$8*FA!$H$8*P14, 0)</f>
         <v>392653</v>
       </c>
@@ -4216,325 +4314,325 @@
         <f t="shared" ref="T14" si="1">DATE(VALUE(RIGHT(D14,4)), IFERROR(VALUE(LEFT(D14,2)), VALUE(LEFT(D14,1))), IFERROR(VALUE(MID(D14,3,2)),VALUE(MID(D14,4,2))))</f>
         <v>45250</v>
       </c>
-      <c r="U14" s="21">
+      <c r="U14" s="36">
         <f t="shared" ref="U14" si="2">IF($T14&lt;$J$9,1,0)*$K$9*P14 + IF($T14&lt;$J$10,1,0)*$K$10*P14 + IF($T14&lt;$J$11,1,0)*$K$11*P14 + IF($T14&lt;$J$8,1,0)*$K$8*P14</f>
         <v>100.5</v>
       </c>
-      <c r="V14" s="21">
+      <c r="V14" s="36">
         <f>ROUND((IF($T14&lt;$J$9,1,0)*$K$9*$L$9 + IF($T14&lt;$J$10,1,0)*$K$10*$L$10 + IF($T14&lt;$J$11,1,0)*$K$11*$L$11 + IF($T14&lt;$J$8,1,0)*$K$8*$L$8)*$P14, 0)</f>
         <v>8373</v>
       </c>
-      <c r="W14" s="21">
+      <c r="W14" s="36">
         <f t="shared" ref="W14" si="3">0.25*V14</f>
         <v>2093.25</v>
       </c>
-      <c r="X14" s="21">
+      <c r="X14" s="36">
         <f t="shared" ref="X14" si="4">0.3132*V14</f>
         <v>2622.4235999999996</v>
       </c>
-      <c r="Y14" s="21">
+      <c r="Y14" s="36">
         <f t="shared" ref="Y14" si="5">X14-W14</f>
         <v>529.17359999999962</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
       <c r="T15" s="17"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
     </row>
     <row r="16" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
       <c r="T16" s="17"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
       <c r="T17" s="17"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
       <c r="T18" s="17"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
       <c r="T19" s="17"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
       <c r="T20" s="17"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
       <c r="T21" s="17"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
       <c r="T22" s="17"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-      <c r="W23"/>
-      <c r="X23"/>
-      <c r="Y23"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="22"/>
+      <c r="Y23" s="22"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-      <c r="W24"/>
-      <c r="X24"/>
-      <c r="Y24"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
+      <c r="W24" s="22"/>
+      <c r="X24" s="22"/>
+      <c r="Y24" s="22"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="43" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25"/>
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
+      <c r="V25" s="22"/>
+      <c r="W25" s="22"/>
+      <c r="X25" s="22"/>
+      <c r="Y25" s="22"/>
     </row>
     <row r="26" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E26" s="3" t="s">
@@ -4607,10 +4705,10 @@
       </c>
       <c r="B27" s="54"/>
       <c r="C27" s="54"/>
-      <c r="E27" s="2">
+      <c r="E27" s="37">
         <v>12312</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="37" t="s">
         <v>134</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -4619,75 +4717,75 @@
       <c r="H27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="37">
         <v>2</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="37">
         <v>112.3445</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="37">
         <v>148.51</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="37">
         <v>41</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="37">
         <v>82.78</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O27" s="37">
         <v>123</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P27" s="37">
         <v>2</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="36">
         <f>ROUND(P27*K27*N27, 0)</f>
         <v>24587</v>
       </c>
-      <c r="R27" s="21">
+      <c r="R27" s="36">
         <v>136422</v>
       </c>
-      <c r="S27" s="21">
+      <c r="S27" s="36">
         <v>0</v>
       </c>
       <c r="T27" s="10">
         <f>DATE(VALUE(RIGHT(H27,4)), IFERROR(VALUE(LEFT(H27,2)), VALUE(LEFT(H27,1))), IFERROR(VALUE(MID(H27,3,2)),VALUE(MID(H27,4,2))))</f>
         <v>45322</v>
       </c>
-      <c r="U27" s="21">
+      <c r="U27" s="36">
         <f>IF($T27&lt;FA!$J$8,1,0)*FA!$K$8*P27</f>
         <v>1.6</v>
       </c>
-      <c r="V27" s="21">
+      <c r="V27" s="36">
         <f>ROUND((IF($T27&lt;FA!$J$8,1,0)*FA!$K$8*FA!$L$8)*$P27, 0)</f>
         <v>132</v>
       </c>
-      <c r="W27" s="21">
+      <c r="W27" s="36">
         <f>0.25*V27</f>
         <v>33</v>
       </c>
-      <c r="X27" s="21">
+      <c r="X27" s="36">
         <f>0.3132*V27</f>
         <v>41.342399999999998</v>
       </c>
-      <c r="Y27" s="21">
+      <c r="Y27" s="36">
         <f>X27-W27</f>
         <v>8.3423999999999978</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="E28" s="2">
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="E28" s="37">
         <v>12312</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="37" t="s">
         <v>134</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -4696,39 +4794,39 @@
       <c r="H28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="37">
         <v>1</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="37">
         <v>112.3445</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="37">
         <v>148.51</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="37">
         <v>12</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M28" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="37">
         <v>82.78</v>
       </c>
-      <c r="O28" s="2">
+      <c r="O28" s="37">
         <v>12312</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="37">
         <v>1</v>
       </c>
-      <c r="Q28" s="28">
+      <c r="Q28" s="36">
         <f>ROUND(P28*K28*N28, 0)</f>
         <v>12294</v>
       </c>
-      <c r="R28" s="28" cm="1">
+      <c r="R28" s="36" cm="1">
         <f t="array" ref="R28">ROUND(_xlfn.LET(_xlpm.peak_after, MATCH(MIN(IF($C$8:$C$12&gt;=T28, $C$8:$C$12)), $C$8:$C$12, 0), INDEX($E$8:$E$12, _xlpm.peak_after) * INDEX($F$8:$F$12, _xlpm.peak_after)) *P28, 0)</f>
         <v>18876</v>
       </c>
-      <c r="S28" s="28">
+      <c r="S28" s="36">
         <f>ROUND(G8*H8*P28, 0)</f>
         <v>13088</v>
       </c>
@@ -4736,262 +4834,228 @@
         <f>DATE(VALUE(RIGHT(H28,4)), IFERROR(VALUE(LEFT(H28,2)), VALUE(LEFT(H28,1))), IFERROR(VALUE(MID(H28,3,2)),VALUE(MID(H28,4,2))))</f>
         <v>45322</v>
       </c>
-      <c r="U28" s="28">
+      <c r="U28" s="36">
         <f>IF($T28&lt;FA!$J$8,1,0)*FA!$K$8*P28 + IF($T28&lt;FA!$J$9,1,0)*FA!$K$9*P28 + IF($T28&lt;FA!$J$10,1,0)*FA!$K$10*P28 + IF($T28&lt;FA!$J$11,1,0)*FA!$K$11*P28</f>
         <v>3.35</v>
       </c>
-      <c r="V28" s="28">
+      <c r="V28" s="36">
         <f>ROUND((IF($T28&lt;FA!$J$8,1,0)*FA!$K$8*FA!$L$8 + IF($T28&lt;FA!$J$9,1,0)*FA!$K$9*FA!$L$9 + IF($T28&lt;FA!$J$10,1,0)*FA!$K$10*FA!$L$10 + IF($T28&lt;FA!$J$11,1,0)*FA!$K$11*FA!$L$11)*$P28, 0)</f>
         <v>279</v>
       </c>
-      <c r="W28" s="28">
+      <c r="W28" s="36">
         <f>0.25*V28</f>
         <v>69.75</v>
       </c>
-      <c r="X28" s="28">
+      <c r="X28" s="36">
         <f>0.3132*V28</f>
         <v>87.382799999999989</v>
       </c>
-      <c r="Y28" s="28">
+      <c r="Y28" s="36">
         <f>X28-W28</f>
         <v>17.632799999999989</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+    </row>
+    <row r="33" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="64"/>
       <c r="Q33" s="15"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="60" t="s">
+    <row r="34" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="B34" s="60"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="61" t="s">
+      <c r="C35" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+    </row>
+    <row r="36" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="40">
-        <f>ROUND(SUM(O17:O25,O31) * D15 * E15, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="55" t="s">
+      <c r="B36" s="38">
+        <f>SUM(S16:S24,S29:S30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="38">
+        <v>100</v>
+      </c>
+      <c r="C37" s="38">
+        <f>SUM(V16:V24,V29:V30)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="40">
-        <f>SUM(R17:R25,R30:R31)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="40">
-        <v>19180</v>
-      </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
+      <c r="B38" s="38">
+        <v>200</v>
+      </c>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="40">
-        <v>136422</v>
-      </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22">
+        <f>SUM(C37,B38)</f>
+        <v>200</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41" s="26"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42" s="26"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43" s="26"/>
-      <c r="H43"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44" s="26"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-      <c r="G45" s="26"/>
-      <c r="H45"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46" s="26"/>
-      <c r="H46"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47" s="26"/>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48" s="26"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C36:I36"/>
     <mergeCell ref="M5:X5"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="E25:P25"/>
@@ -5002,6 +5066,8 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="M1:T3"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C35:F35"/>
   </mergeCells>
   <conditionalFormatting sqref="X11">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
@@ -5030,7 +5096,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5045,119 +5111,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
+      <c r="C4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
+      <c r="C5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
     </row>
     <row r="6" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="C6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
+      <c r="A6" s="24"/>
+      <c r="C6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="E7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="57" t="s">
+      <c r="C7" s="27"/>
+      <c r="E7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="E8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="57" t="s">
+      <c r="C8" s="27"/>
+      <c r="E8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
+      <c r="C9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="C10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
+      <c r="A10" s="24"/>
+      <c r="C10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="C11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="58" t="s">
         <v>126</v>
       </c>
@@ -5165,154 +5231,153 @@
       <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
+      <c r="C12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="C13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
+      <c r="A13" s="24"/>
+      <c r="C13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="57" t="s">
+      <c r="C14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="57" t="s">
+      <c r="C15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
+      <c r="C16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="57" t="s">
+      <c r="C17" s="27"/>
+      <c r="E17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="57" t="s">
+      <c r="C18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="57" t="s">
+      <c r="C19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="C20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
+      <c r="A20" s="24"/>
+      <c r="C20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
+      <c r="C21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
     </row>
     <row r="22" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
+      <c r="C22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="E23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="57" t="s">
+      <c r="C23" s="27"/>
+      <c r="E23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
@@ -5325,11 +5390,12 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>